<commit_message>
new figures and analyses
added rfx analyses
fixed bubble plots so that normalized sizes make sense
added mds code
</commit_message>
<xml_diff>
--- a/letter similarity stuff/Non-Gibson Letter Distances.xlsx
+++ b/letter similarity stuff/Non-Gibson Letter Distances.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="376">
   <si>
     <t>LetterPairIndex</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1072,19 +1072,128 @@
   </si>
   <si>
     <t>EaglemanRGBdists</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>letters</t>
+  </si>
+  <si>
+    <t>lewand frequency</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>diff/sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -1105,15 +1214,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1441,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T326"/>
+  <dimension ref="A1:AA326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1459,9 +1579,10 @@
     <col min="9" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="13.85546875" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1522,8 +1643,23 @@
       <c r="T1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="V1" t="s">
+        <v>371</v>
+      </c>
+      <c r="W1" t="s">
+        <v>372</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>373</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1586,8 +1722,26 @@
       <c r="T2">
         <v>0.87163000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="V2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="W2">
+        <v>8.1670000000000006E-2</v>
+      </c>
+      <c r="Y2">
+        <f>W2+W3</f>
+        <v>9.6590000000000009E-2</v>
+      </c>
+      <c r="Z2">
+        <f>W2-W3</f>
+        <v>6.6750000000000004E-2</v>
+      </c>
+      <c r="AA2">
+        <f>Z2/Y2</f>
+        <v>0.69106532767367224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1650,8 +1804,14 @@
       <c r="T3">
         <v>0.85372000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="V3" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="W3">
+        <v>1.4919999999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1714,8 +1874,14 @@
       <c r="T4">
         <v>0.79634000000000005</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="V4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="W4">
+        <v>2.7820000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1778,8 +1944,14 @@
       <c r="T5">
         <v>0.83933000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="V5" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="W5">
+        <v>4.2529999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1842,8 +2014,14 @@
       <c r="T6">
         <v>0.77202000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="V6" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="W6">
+        <v>0.12701999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1906,8 +2084,14 @@
       <c r="T7">
         <v>0.77151999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="V7" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="W7">
+        <v>2.2280000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1970,8 +2154,14 @@
       <c r="T8">
         <v>0.71143000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="V8" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="W8">
+        <v>2.0150000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2034,8 +2224,14 @@
       <c r="T9">
         <v>0.96231</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="V9" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="W9">
+        <v>6.0940000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2098,8 +2294,14 @@
       <c r="T10">
         <v>0.79181000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="V10" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="W10">
+        <v>6.966E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2162,8 +2364,14 @@
       <c r="T11">
         <v>0.73726000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="V11" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="W11">
+        <v>1.5299999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2226,8 +2434,14 @@
       <c r="T12">
         <v>0.84702</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="V12" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="W12">
+        <v>7.7200000000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2290,8 +2504,14 @@
       <c r="T13">
         <v>0.72787999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="V13" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="W13">
+        <v>4.0250000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2354,8 +2574,14 @@
       <c r="T14">
         <v>0.74294000000000004</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="V14" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="W14">
+        <v>2.4060000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2418,8 +2644,14 @@
       <c r="T15">
         <v>0.93896000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="V15" t="s">
+        <v>346</v>
+      </c>
+      <c r="W15">
+        <v>6.7489999999999994E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2482,8 +2714,14 @@
       <c r="T16">
         <v>0.78139999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="V16" t="s">
+        <v>348</v>
+      </c>
+      <c r="W16">
+        <v>7.5069999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2546,8 +2784,14 @@
       <c r="T17">
         <v>0.80845999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="V17" t="s">
+        <v>350</v>
+      </c>
+      <c r="W17">
+        <v>1.9290000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2610,8 +2854,14 @@
       <c r="T18">
         <v>0.68145999999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="V18" t="s">
+        <v>352</v>
+      </c>
+      <c r="W18">
+        <v>9.5E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2674,8 +2924,14 @@
       <c r="T19">
         <v>0.80820999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="V19" t="s">
+        <v>354</v>
+      </c>
+      <c r="W19">
+        <v>5.987E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2738,8 +2994,14 @@
       <c r="T20">
         <v>0.81055999999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="V20" t="s">
+        <v>356</v>
+      </c>
+      <c r="W20">
+        <v>6.3270000000000007E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2802,8 +3064,14 @@
       <c r="T21">
         <v>0.80171999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:20">
+      <c r="V21" t="s">
+        <v>358</v>
+      </c>
+      <c r="W21">
+        <v>9.0560000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2866,8 +3134,14 @@
       <c r="T22">
         <v>0.77751999999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
+      <c r="V22" t="s">
+        <v>360</v>
+      </c>
+      <c r="W22">
+        <v>2.758E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2930,8 +3204,14 @@
       <c r="T23">
         <v>0.83038999999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:20">
+      <c r="V23" t="s">
+        <v>362</v>
+      </c>
+      <c r="W23">
+        <v>9.7800000000000005E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2994,8 +3274,14 @@
       <c r="T24">
         <v>0.80862000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="V24" t="s">
+        <v>364</v>
+      </c>
+      <c r="W24">
+        <v>2.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3058,8 +3344,14 @@
       <c r="T25">
         <v>0.77873999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:20">
+      <c r="V25" t="s">
+        <v>366</v>
+      </c>
+      <c r="W25">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3122,8 +3414,14 @@
       <c r="T26">
         <v>0.82777000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:20">
+      <c r="V26" t="s">
+        <v>368</v>
+      </c>
+      <c r="W26">
+        <v>1.9740000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3186,8 +3484,14 @@
       <c r="T27">
         <v>0.89159999999999995</v>
       </c>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="V27" t="s">
+        <v>370</v>
+      </c>
+      <c r="W27">
+        <v>7.3999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3251,7 +3555,7 @@
         <v>0.67142999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:23">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3315,7 +3619,7 @@
         <v>0.81462000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:23">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3379,7 +3683,7 @@
         <v>0.75307000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:23">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3443,7 +3747,7 @@
         <v>0.69023999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:23">
       <c r="A32">
         <v>31</v>
       </c>
@@ -22326,6 +22630,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
figures and english word count data
-nans vs. letter frequencies
-added word counts for english from google db
-added letter frequencies from google db
-minor edits to main script
</commit_message>
<xml_diff>
--- a/letter similarity stuff/Non-Gibson Letter Distances.xlsx
+++ b/letter similarity stuff/Non-Gibson Letter Distances.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="11220" yWindow="0" windowWidth="15540" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="377">
   <si>
     <t>LetterPairIndex</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1165,6 +1165,9 @@
   </si>
   <si>
     <t>diff/sum</t>
+  </si>
+  <si>
+    <t>fq from google database</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1217,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1229,11 +1240,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1561,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA326"/>
+  <dimension ref="A1:AC326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AC31" sqref="AC31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1582,7 +1601,7 @@
     <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1658,8 +1677,11 @@
       <c r="AA1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="2" spans="1:27">
+      <c r="AC1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1740,8 +1762,14 @@
         <f>Z2/Y2</f>
         <v>0.69106532767367224</v>
       </c>
-    </row>
-    <row r="3" spans="1:27">
+      <c r="AB2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="AC2">
+        <v>8.0399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1810,8 +1838,14 @@
       <c r="W3">
         <v>1.4919999999999999E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27">
+      <c r="AB3" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AC3">
+        <v>1.4800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1880,8 +1914,14 @@
       <c r="W4">
         <v>2.7820000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27">
+      <c r="AB4" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="AC4">
+        <v>3.3399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1950,8 +1990,14 @@
       <c r="W5">
         <v>4.2529999999999998E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:27">
+      <c r="AB5" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="AC5">
+        <v>3.8199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2020,8 +2066,14 @@
       <c r="W6">
         <v>0.12701999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:27">
+      <c r="AB6" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="AC6">
+        <v>0.1249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2090,8 +2142,14 @@
       <c r="W7">
         <v>2.2280000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:27">
+      <c r="AB7" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="AC7">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2160,8 +2218,14 @@
       <c r="W8">
         <v>2.0150000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:27">
+      <c r="AB8" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="AC8">
+        <v>1.8700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2230,8 +2294,14 @@
       <c r="W9">
         <v>6.0940000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:27">
+      <c r="AB9" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC9">
+        <v>5.0500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2300,8 +2370,14 @@
       <c r="W10">
         <v>6.966E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:27">
+      <c r="AB10" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="AC10">
+        <v>7.5700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2370,8 +2446,14 @@
       <c r="W11">
         <v>1.5299999999999999E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:27">
+      <c r="AB11" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="AC11">
+        <v>1.6000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2440,8 +2522,14 @@
       <c r="W12">
         <v>7.7200000000000003E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:27">
+      <c r="AB12" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="AC12">
+        <v>5.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2510,8 +2598,14 @@
       <c r="W13">
         <v>4.0250000000000001E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:27">
+      <c r="AB13" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="AC13">
+        <v>4.07E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2580,8 +2674,14 @@
       <c r="W14">
         <v>2.4060000000000002E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:27">
+      <c r="AB14" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AC14">
+        <v>2.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2650,8 +2750,14 @@
       <c r="W15">
         <v>6.7489999999999994E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:27">
+      <c r="AB15" t="s">
+        <v>346</v>
+      </c>
+      <c r="AC15">
+        <v>7.2300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2720,8 +2826,14 @@
       <c r="W16">
         <v>7.5069999999999998E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:23">
+      <c r="AB16" t="s">
+        <v>348</v>
+      </c>
+      <c r="AC16">
+        <v>7.6399999999999996E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2790,8 +2902,14 @@
       <c r="W17">
         <v>1.9290000000000002E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:23">
+      <c r="AB17" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC17">
+        <v>2.1399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2860,8 +2978,14 @@
       <c r="W18">
         <v>9.5E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:23">
+      <c r="AB18" t="s">
+        <v>352</v>
+      </c>
+      <c r="AC18">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2930,8 +3054,14 @@
       <c r="W19">
         <v>5.987E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:23">
+      <c r="AB19" t="s">
+        <v>354</v>
+      </c>
+      <c r="AC19">
+        <v>6.2799999999999995E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3000,8 +3130,14 @@
       <c r="W20">
         <v>6.3270000000000007E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:23">
+      <c r="AB20" t="s">
+        <v>356</v>
+      </c>
+      <c r="AC20">
+        <v>6.5100000000000005E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3070,8 +3206,14 @@
       <c r="W21">
         <v>9.0560000000000002E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:23">
+      <c r="AB21" t="s">
+        <v>358</v>
+      </c>
+      <c r="AC21">
+        <v>9.2799999999999994E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3140,8 +3282,14 @@
       <c r="W22">
         <v>2.758E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:23">
+      <c r="AB22" t="s">
+        <v>360</v>
+      </c>
+      <c r="AC22">
+        <v>2.7300000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3210,8 +3358,14 @@
       <c r="W23">
         <v>9.7800000000000005E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:23">
+      <c r="AB23" t="s">
+        <v>362</v>
+      </c>
+      <c r="AC23">
+        <v>1.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3280,8 +3434,14 @@
       <c r="W24">
         <v>2.3599999999999999E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:23">
+      <c r="AB24" t="s">
+        <v>364</v>
+      </c>
+      <c r="AC24">
+        <v>1.6799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3350,8 +3510,14 @@
       <c r="W25">
         <v>1.5E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:23">
+      <c r="AB25" t="s">
+        <v>366</v>
+      </c>
+      <c r="AC25">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3420,8 +3586,14 @@
       <c r="W26">
         <v>1.9740000000000001E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:23">
+      <c r="AB26" t="s">
+        <v>368</v>
+      </c>
+      <c r="AC26">
+        <v>1.66E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3490,8 +3662,14 @@
       <c r="W27">
         <v>7.3999999999999999E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:23">
+      <c r="AB27" t="s">
+        <v>370</v>
+      </c>
+      <c r="AC27">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3554,8 +3732,16 @@
       <c r="T28">
         <v>0.67142999999999997</v>
       </c>
-    </row>
-    <row r="29" spans="1:23">
+      <c r="W28">
+        <f>SUM(W2:W27)</f>
+        <v>0.99998999999999982</v>
+      </c>
+      <c r="AC28">
+        <f>SUM(AC2:AC27)</f>
+        <v>0.99979999999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3619,7 +3805,7 @@
         <v>0.81462000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:29">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3683,7 +3869,7 @@
         <v>0.75307000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:29">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3747,7 +3933,7 @@
         <v>0.69023999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:29">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>